<commit_message>
display GUI and calculations
</commit_message>
<xml_diff>
--- a/Submission 2.0/i75_error_log.xlsx
+++ b/Submission 2.0/i75_error_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msais\Desktop\Submission2.0\Submission 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF52CB0A-B7D7-43C7-8823-72B1D7B4BA98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF7CBE5-ADED-403F-AAA9-1FDD90B97A9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BA761C28-96FE-464C-ACD2-9DE5B797B113}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,10 +540,10 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>736512.24057553802</v>
+        <v>736482.01721401198</v>
       </c>
       <c r="D5">
-        <v>3750779.9964897898</v>
+        <v>3750779.9454453602</v>
       </c>
       <c r="E5">
         <v>736465.73748737096</v>

</xml_diff>